<commit_message>
new run of the fim
</commit_message>
<xml_diff>
--- a/results/07-2023/comparison-deflators-07-2023.xlsx
+++ b/results/07-2023/comparison-deflators-07-2023.xlsx
@@ -1236,28 +1236,28 @@
         <v>0</v>
       </c>
       <c r="L13" t="n">
-        <v>0.0437</v>
+        <v>0.0044</v>
       </c>
       <c r="M13" t="n">
-        <v>0.0313</v>
+        <v>0.0031</v>
       </c>
       <c r="N13" t="n">
-        <v>0.0406</v>
+        <v>0.0041</v>
       </c>
       <c r="O13" t="n">
-        <v>0.022</v>
+        <v>0.0022</v>
       </c>
       <c r="P13" t="n">
-        <v>0.0217</v>
+        <v>0.0022</v>
       </c>
       <c r="Q13" t="n">
-        <v>0.0181</v>
+        <v>0.0018</v>
       </c>
       <c r="R13" t="n">
-        <v>0.0173</v>
+        <v>0.0017</v>
       </c>
       <c r="S13" t="n">
-        <v>-0.0353</v>
+        <v>-0.0035</v>
       </c>
     </row>
     <row r="14">
@@ -1413,28 +1413,28 @@
         <v>-0.7403</v>
       </c>
       <c r="L16" t="n">
-        <v>-0.2652</v>
+        <v>-0.3045</v>
       </c>
       <c r="M16" t="n">
-        <v>-0.2644</v>
+        <v>-0.2926</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.5113</v>
+        <v>-0.5478</v>
       </c>
       <c r="O16" t="n">
-        <v>0.0023</v>
+        <v>-0.0175</v>
       </c>
       <c r="P16" t="n">
-        <v>-0.0469</v>
+        <v>-0.0664</v>
       </c>
       <c r="Q16" t="n">
-        <v>0.074</v>
+        <v>0.0577</v>
       </c>
       <c r="R16" t="n">
-        <v>-0.0566</v>
+        <v>-0.0722</v>
       </c>
       <c r="S16" t="n">
-        <v>-72.7416</v>
+        <v>-72.7098</v>
       </c>
     </row>
     <row r="17">
@@ -2888,28 +2888,28 @@
         <v>0</v>
       </c>
       <c r="L41" t="n">
-        <v>0</v>
+        <v>-0.0393</v>
       </c>
       <c r="M41" t="n">
-        <v>0.0005</v>
+        <v>-0.0277</v>
       </c>
       <c r="N41" t="n">
-        <v>0.0006</v>
+        <v>-0.0359</v>
       </c>
       <c r="O41" t="n">
-        <v>0.0003</v>
+        <v>-0.0195</v>
       </c>
       <c r="P41" t="n">
-        <v>0.0003</v>
+        <v>-0.0192</v>
       </c>
       <c r="Q41" t="n">
-        <v>0.0002</v>
+        <v>-0.016</v>
       </c>
       <c r="R41" t="n">
-        <v>0.0002</v>
+        <v>-0.0153</v>
       </c>
       <c r="S41" t="n">
-        <v>-0.0006</v>
+        <v>0.0312</v>
       </c>
     </row>
     <row r="42">
@@ -3065,28 +3065,28 @@
         <v>0.342</v>
       </c>
       <c r="L44" t="n">
-        <v>-0.1507</v>
+        <v>-0.19</v>
       </c>
       <c r="M44" t="n">
-        <v>-0.0314</v>
+        <v>-0.0595</v>
       </c>
       <c r="N44" t="n">
-        <v>-0.0531</v>
+        <v>-0.0897</v>
       </c>
       <c r="O44" t="n">
-        <v>0.0963</v>
+        <v>0.0765</v>
       </c>
       <c r="P44" t="n">
-        <v>-0.0375</v>
+        <v>-0.057</v>
       </c>
       <c r="Q44" t="n">
-        <v>-0.0324</v>
+        <v>-0.0487</v>
       </c>
       <c r="R44" t="n">
-        <v>-0.0263</v>
+        <v>-0.0418</v>
       </c>
       <c r="S44" t="n">
-        <v>-1.0301</v>
+        <v>-0.9983</v>
       </c>
     </row>
     <row r="45">

</xml_diff>